<commit_message>
Update Outputs of all models.xlsx
</commit_message>
<xml_diff>
--- a/Outputs of all models.xlsx
+++ b/Outputs of all models.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JingYuan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JingYuan\Desktop\All\Dataset-and-predicted-results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29EEB885-C5AC-43EC-99C0-E825DA95403F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D468420B-4F8A-4B89-A8FE-488509D3D48B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Outputs of c" sheetId="6" r:id="rId1"/>
@@ -115,9 +115,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Actual φ (°)</t>
-  </si>
-  <si>
     <t>Rock type</t>
   </si>
   <si>
@@ -167,6 +164,10 @@
   </si>
   <si>
     <t>Quartz mica schist</t>
+  </si>
+  <si>
+    <t>Actual c (MPa)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -514,77 +515,77 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB63BE65-DED5-4E0E-9099-0A4CDD5B5A75}">
   <dimension ref="A1:P200"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="14.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="16" width="14.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16" width="12.77734375" style="2" bestFit="1" customWidth="1"/>
     <col min="17" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" s="2">
         <v>5065.12</v>
@@ -2937,7 +2938,7 @@
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B52" s="2">
         <v>3487.25</v>
@@ -9957,7 +9958,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE5BB38B-42F1-4A35-B023-79648DD9ED00}">
   <dimension ref="A1:P200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>

</xml_diff>